<commit_message>
updated dashboard and codes
</commit_message>
<xml_diff>
--- a/data_total.xlsx
+++ b/data_total.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data science 2025\git_repository\data-science-project-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CB050D-130E-468E-9241-24CC3FCF97A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9744F4-52E7-4C1C-AC8A-CA51CDDBCC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6796A59-E328-4143-AF9C-DD0BC3AEC6A0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E6796A59-E328-4143-AF9C-DD0BC3AEC6A0}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="99">
   <si>
     <t>Country</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>datascience</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>search index</t>
   </si>
 </sst>
 </file>
@@ -1158,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418E3F93-9535-4EE4-8DBC-8D5F630A4990}">
   <dimension ref="A1:C342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
+    <sheetView topLeftCell="A318" workbookViewId="0">
       <selection activeCell="A279" sqref="A279:D342"/>
     </sheetView>
   </sheetViews>
@@ -4933,31 +4939,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEA6E78-5ACB-42CC-933F-2CDDC2A6B95D}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="B2">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>96</v>
@@ -4965,10 +4971,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B3">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
         <v>96</v>
@@ -4976,10 +4982,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
         <v>96</v>
@@ -4987,10 +4993,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
         <v>96</v>
@@ -4998,10 +5004,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B6">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
         <v>96</v>
@@ -5009,7 +5015,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>63</v>
@@ -5020,10 +5026,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
         <v>96</v>
@@ -5031,10 +5037,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
         <v>96</v>
@@ -5042,7 +5048,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>58</v>
@@ -5053,10 +5059,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
         <v>96</v>
@@ -5064,10 +5070,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B12">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
         <v>96</v>
@@ -5075,10 +5081,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
         <v>96</v>
@@ -5086,10 +5092,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>96</v>
@@ -5097,10 +5103,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>36</v>
       </c>
       <c r="B15">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
         <v>96</v>
@@ -5108,10 +5114,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B16">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
         <v>96</v>
@@ -5119,10 +5125,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="B17">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
         <v>96</v>
@@ -5130,10 +5136,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="B18">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>96</v>
@@ -5141,7 +5147,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="B19">
         <v>27</v>
@@ -5152,10 +5158,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B20">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
         <v>96</v>
@@ -5163,10 +5169,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B21">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
         <v>96</v>
@@ -5174,7 +5180,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B22">
         <v>25</v>
@@ -5185,7 +5191,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B23">
         <v>25</v>
@@ -5196,7 +5202,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B24">
         <v>25</v>
@@ -5207,7 +5213,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="B25">
         <v>25</v>
@@ -5218,10 +5224,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B26">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
         <v>96</v>
@@ -5229,10 +5235,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B27">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
         <v>96</v>
@@ -5240,10 +5246,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B28">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
         <v>96</v>
@@ -5251,7 +5257,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="B29">
         <v>18</v>
@@ -5262,7 +5268,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>18</v>
@@ -5273,10 +5279,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B31">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
         <v>96</v>
@@ -5284,10 +5290,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="B32">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C32" t="s">
         <v>96</v>
@@ -5295,10 +5301,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B33">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
         <v>96</v>
@@ -5306,10 +5312,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B34">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s">
         <v>96</v>
@@ -5317,10 +5323,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="B35">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
         <v>96</v>
@@ -5328,7 +5334,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B36">
         <v>13</v>
@@ -5339,10 +5345,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="B37">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
         <v>96</v>
@@ -5350,7 +5356,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B38">
         <v>12</v>
@@ -5361,7 +5367,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B39">
         <v>12</v>
@@ -5372,7 +5378,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="B40">
         <v>12</v>
@@ -5383,10 +5389,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="B41">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
         <v>96</v>
@@ -5394,10 +5400,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="B42">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C42" t="s">
         <v>96</v>
@@ -5405,7 +5411,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="B43">
         <v>10</v>
@@ -5416,7 +5422,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="B44">
         <v>10</v>
@@ -5427,7 +5433,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B45">
         <v>10</v>
@@ -5438,7 +5444,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="B46">
         <v>10</v>
@@ -5449,7 +5455,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="B47">
         <v>10</v>
@@ -5460,7 +5466,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="B48">
         <v>10</v>
@@ -5471,10 +5477,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B49">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C49" t="s">
         <v>96</v>
@@ -5482,7 +5488,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B50">
         <v>9</v>
@@ -5493,7 +5499,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B51">
         <v>9</v>
@@ -5504,7 +5510,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B52">
         <v>9</v>
@@ -5515,7 +5521,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B53">
         <v>9</v>
@@ -5526,7 +5532,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B54">
         <v>9</v>
@@ -5537,10 +5543,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="B55">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C55" t="s">
         <v>96</v>
@@ -5548,10 +5554,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="B56">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C56" t="s">
         <v>96</v>
@@ -5559,7 +5565,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="B57">
         <v>7</v>
@@ -5570,10 +5576,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B58">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C58" t="s">
         <v>96</v>
@@ -5581,7 +5587,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B59">
         <v>6</v>
@@ -5592,7 +5598,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B60">
         <v>6</v>
@@ -5603,7 +5609,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B61">
         <v>6</v>
@@ -5614,10 +5620,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B62">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C62" t="s">
         <v>96</v>
@@ -5625,10 +5631,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="B63">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
         <v>96</v>
@@ -5636,12 +5642,23 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>88</v>
       </c>
-      <c r="B64">
+      <c r="B65">
         <v>2</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>96</v>
       </c>
     </row>
@@ -5652,31 +5669,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B82A23-4C40-4347-9E65-4B9233E54A84}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D61"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>94</v>
@@ -5684,10 +5701,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="B3">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
         <v>94</v>
@@ -5695,10 +5712,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
         <v>94</v>
@@ -5706,7 +5723,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5">
         <v>48</v>
@@ -5717,10 +5734,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="B6">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
         <v>94</v>
@@ -5728,10 +5745,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="B7">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
         <v>94</v>
@@ -5739,10 +5756,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B8">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
         <v>94</v>
@@ -5750,10 +5767,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>94</v>
@@ -5761,10 +5778,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B10">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
         <v>94</v>
@@ -5772,10 +5789,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B11">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
         <v>94</v>
@@ -5783,10 +5800,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
         <v>94</v>
@@ -5794,10 +5811,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
         <v>94</v>
@@ -5805,10 +5822,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="B14">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
         <v>94</v>
@@ -5816,10 +5833,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B15">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>94</v>
@@ -5827,7 +5844,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B16">
         <v>24</v>
@@ -5838,10 +5855,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B17">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>94</v>
@@ -5849,7 +5866,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>22</v>
@@ -5860,7 +5877,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>22</v>
@@ -5871,10 +5888,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B20">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
         <v>94</v>
@@ -5882,10 +5899,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>94</v>
@@ -5893,7 +5910,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="B22">
         <v>20</v>
@@ -5904,10 +5921,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="B23">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
         <v>94</v>
@@ -5915,7 +5932,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B24">
         <v>19</v>
@@ -5926,10 +5943,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B25">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
         <v>94</v>
@@ -5937,7 +5954,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B26">
         <v>18</v>
@@ -5948,7 +5965,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="B27">
         <v>18</v>
@@ -5959,10 +5976,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B28">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
         <v>94</v>
@@ -5970,7 +5987,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B29">
         <v>17</v>
@@ -5981,7 +5998,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B30">
         <v>17</v>
@@ -5992,10 +6009,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B31">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
         <v>94</v>
@@ -6003,10 +6020,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B32">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
         <v>94</v>
@@ -6014,7 +6031,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="B33">
         <v>15</v>
@@ -6025,10 +6042,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B34">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s">
         <v>94</v>
@@ -6036,7 +6053,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B35">
         <v>14</v>
@@ -6047,7 +6064,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B36">
         <v>14</v>
@@ -6058,10 +6075,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B37">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
         <v>94</v>
@@ -6069,7 +6086,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B38">
         <v>13</v>
@@ -6080,10 +6097,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B39">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C39" t="s">
         <v>94</v>
@@ -6091,7 +6108,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40">
         <v>11</v>
@@ -6102,7 +6119,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B41">
         <v>11</v>
@@ -6113,7 +6130,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B42">
         <v>11</v>
@@ -6124,7 +6141,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B43">
         <v>11</v>
@@ -6135,7 +6152,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B44">
         <v>11</v>
@@ -6146,7 +6163,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B45">
         <v>11</v>
@@ -6157,7 +6174,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B46">
         <v>11</v>
@@ -6168,7 +6185,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B47">
         <v>11</v>
@@ -6179,10 +6196,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B48">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C48" t="s">
         <v>94</v>
@@ -6190,7 +6207,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="B49">
         <v>10</v>
@@ -6201,10 +6218,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B50">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C50" t="s">
         <v>94</v>
@@ -6212,7 +6229,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="B51">
         <v>8</v>
@@ -6223,10 +6240,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="B52">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C52" t="s">
         <v>94</v>
@@ -6234,10 +6251,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="B53">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
         <v>94</v>
@@ -6245,7 +6262,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="B54">
         <v>5</v>
@@ -6256,7 +6273,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B55">
         <v>5</v>
@@ -6267,7 +6284,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="B56">
         <v>5</v>
@@ -6278,7 +6295,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B57">
         <v>5</v>
@@ -6289,7 +6306,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="B58">
         <v>5</v>
@@ -6300,7 +6317,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B59">
         <v>5</v>
@@ -6311,10 +6328,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="B60">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
         <v>94</v>
@@ -6322,12 +6339,23 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>87</v>
       </c>
-      <c r="B61">
+      <c r="B62">
         <v>2</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>94</v>
       </c>
     </row>
@@ -6338,31 +6366,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A73716D-A332-4001-B9A5-29FAF891F2E4}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C67"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>91</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>91</v>
@@ -6370,10 +6398,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B3">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>91</v>
@@ -6381,10 +6409,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="B4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>91</v>
@@ -6392,10 +6420,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B5">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>91</v>
@@ -6403,10 +6431,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>91</v>
@@ -6414,10 +6442,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B7">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
         <v>91</v>
@@ -6425,10 +6453,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>91</v>
@@ -6436,7 +6464,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="B9">
         <v>21</v>
@@ -6447,10 +6475,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>91</v>
@@ -6458,7 +6486,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>20</v>
@@ -6469,10 +6497,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>91</v>
@@ -6480,10 +6508,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>91</v>
@@ -6491,10 +6519,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
         <v>91</v>
@@ -6502,7 +6530,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -6513,7 +6541,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>14</v>
@@ -6524,10 +6552,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
         <v>91</v>
@@ -6535,7 +6563,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B18">
         <v>13</v>
@@ -6546,7 +6574,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>13</v>
@@ -6557,7 +6585,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B20">
         <v>13</v>
@@ -6568,7 +6596,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="B21">
         <v>13</v>
@@ -6579,7 +6607,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>13</v>
@@ -6590,10 +6618,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
         <v>91</v>
@@ -6601,10 +6629,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
         <v>91</v>
@@ -6612,7 +6640,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="B25">
         <v>11</v>
@@ -6623,7 +6651,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="B26">
         <v>11</v>
@@ -6634,10 +6662,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
         <v>91</v>
@@ -6645,7 +6673,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B28">
         <v>10</v>
@@ -6656,7 +6684,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B29">
         <v>10</v>
@@ -6667,7 +6695,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B30">
         <v>10</v>
@@ -6678,7 +6706,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B31">
         <v>10</v>
@@ -6689,7 +6717,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="B32">
         <v>10</v>
@@ -6700,10 +6728,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B33">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
         <v>91</v>
@@ -6711,7 +6739,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="B34">
         <v>9</v>
@@ -6722,7 +6750,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B35">
         <v>9</v>
@@ -6733,10 +6761,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="B36">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
         <v>91</v>
@@ -6744,7 +6772,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -6755,7 +6783,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>8</v>
@@ -6766,7 +6794,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="B39">
         <v>8</v>
@@ -6777,7 +6805,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -6788,7 +6816,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="B41">
         <v>8</v>
@@ -6799,10 +6827,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C42" t="s">
         <v>91</v>
@@ -6810,7 +6838,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B43">
         <v>7</v>
@@ -6821,7 +6849,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B44">
         <v>7</v>
@@ -6832,7 +6860,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B45">
         <v>7</v>
@@ -6843,7 +6871,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B46">
         <v>7</v>
@@ -6854,10 +6882,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
         <v>91</v>
@@ -6865,7 +6893,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B48">
         <v>6</v>
@@ -6876,7 +6904,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B49">
         <v>6</v>
@@ -6887,7 +6915,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="B50">
         <v>6</v>
@@ -6898,7 +6926,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B51">
         <v>6</v>
@@ -6909,7 +6937,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B52">
         <v>6</v>
@@ -6920,7 +6948,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B53">
         <v>6</v>
@@ -6931,7 +6959,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="B54">
         <v>6</v>
@@ -6942,10 +6970,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B55">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
         <v>91</v>
@@ -6953,7 +6981,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B56">
         <v>5</v>
@@ -6964,7 +6992,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B57">
         <v>5</v>
@@ -6975,7 +7003,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="B58">
         <v>5</v>
@@ -6986,7 +7014,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="B59">
         <v>5</v>
@@ -6997,7 +7025,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="B60">
         <v>5</v>
@@ -7008,7 +7036,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B61">
         <v>5</v>
@@ -7019,10 +7047,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="B62">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
         <v>91</v>
@@ -7030,7 +7058,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B63">
         <v>4</v>
@@ -7041,7 +7069,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B64">
         <v>4</v>
@@ -7052,10 +7080,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C65" t="s">
         <v>91</v>
@@ -7063,7 +7091,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -7074,12 +7102,23 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="B67">
         <v>3</v>
       </c>
       <c r="C67" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>89</v>
+      </c>
+      <c r="B68">
+        <v>3</v>
+      </c>
+      <c r="C68" t="s">
         <v>91</v>
       </c>
     </row>
@@ -7090,31 +7129,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{979E0FA8-2499-47AA-9C3E-DA5BE38F6C7D}">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C87"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -7122,10 +7161,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -7133,10 +7172,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -7144,10 +7183,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7155,10 +7194,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7166,10 +7205,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -7177,7 +7216,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>70</v>
@@ -7188,10 +7227,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -7199,10 +7238,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7210,10 +7249,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7221,10 +7260,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -7232,10 +7271,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7243,7 +7282,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>59</v>
@@ -7254,10 +7293,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7265,10 +7304,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -7276,7 +7315,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>54</v>
@@ -7287,10 +7326,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -7298,10 +7337,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -7309,7 +7348,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>52</v>
@@ -7320,10 +7359,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -7331,7 +7370,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>51</v>
@@ -7342,10 +7381,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -7353,10 +7392,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -7364,7 +7403,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>47</v>
@@ -7375,7 +7414,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>47</v>
@@ -7386,10 +7425,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -7397,10 +7436,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -7408,10 +7447,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -7419,7 +7458,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>42</v>
@@ -7430,10 +7469,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -7441,10 +7480,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -7452,7 +7491,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>38</v>
@@ -7463,7 +7502,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>38</v>
@@ -7474,10 +7513,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
         <v>38</v>
-      </c>
-      <c r="B35">
-        <v>37</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -7485,10 +7524,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -7496,10 +7535,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -7507,7 +7546,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38">
         <v>32</v>
@@ -7518,10 +7557,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
@@ -7529,7 +7568,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40">
         <v>30</v>
@@ -7540,10 +7579,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -7551,7 +7590,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42">
         <v>29</v>
@@ -7562,7 +7601,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43">
         <v>29</v>
@@ -7573,7 +7612,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44">
         <v>29</v>
@@ -7584,10 +7623,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
@@ -7595,10 +7634,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
@@ -7606,7 +7645,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47">
         <v>27</v>
@@ -7617,7 +7656,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <v>27</v>
@@ -7628,7 +7667,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49">
         <v>27</v>
@@ -7639,10 +7678,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C50" t="s">
         <v>4</v>
@@ -7650,7 +7689,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51">
         <v>25</v>
@@ -7661,10 +7700,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C52" t="s">
         <v>4</v>
@@ -7672,10 +7711,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B53">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C53" t="s">
         <v>4</v>
@@ -7683,7 +7722,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B54">
         <v>23</v>
@@ -7694,10 +7733,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C55" t="s">
         <v>4</v>
@@ -7705,7 +7744,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56">
         <v>21</v>
@@ -7716,7 +7755,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B57">
         <v>21</v>
@@ -7727,10 +7766,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B58">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C58" t="s">
         <v>4</v>
@@ -7738,10 +7777,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B59">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C59" t="s">
         <v>4</v>
@@ -7749,7 +7788,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B60">
         <v>19</v>
@@ -7760,7 +7799,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B61">
         <v>19</v>
@@ -7771,10 +7810,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B62">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
@@ -7782,7 +7821,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B63">
         <v>18</v>
@@ -7793,7 +7832,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B64">
         <v>18</v>
@@ -7804,7 +7843,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B65">
         <v>18</v>
@@ -7815,7 +7854,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66">
         <v>18</v>
@@ -7826,7 +7865,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B67">
         <v>18</v>
@@ -7837,7 +7876,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B68">
         <v>18</v>
@@ -7848,10 +7887,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B69">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C69" t="s">
         <v>4</v>
@@ -7859,10 +7898,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B70">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C70" t="s">
         <v>4</v>
@@ -7870,7 +7909,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B71">
         <v>16</v>
@@ -7881,10 +7920,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B72">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C72" t="s">
         <v>4</v>
@@ -7892,7 +7931,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B73">
         <v>15</v>
@@ -7903,10 +7942,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B74">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C74" t="s">
         <v>4</v>
@@ -7914,7 +7953,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75">
         <v>14</v>
@@ -7925,7 +7964,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B76">
         <v>14</v>
@@ -7936,7 +7975,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B77">
         <v>14</v>
@@ -7947,10 +7986,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C78" t="s">
         <v>4</v>
@@ -7958,10 +7997,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B79">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C79" t="s">
         <v>4</v>
@@ -7969,7 +8008,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B80">
         <v>12</v>
@@ -7980,10 +8019,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B81">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C81" t="s">
         <v>4</v>
@@ -7991,7 +8030,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B82">
         <v>11</v>
@@ -8002,10 +8041,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B83">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C83" t="s">
         <v>4</v>
@@ -8013,10 +8052,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B84">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C84" t="s">
         <v>4</v>
@@ -8024,10 +8063,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B85">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C85" t="s">
         <v>4</v>
@@ -8035,7 +8074,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B86">
         <v>7</v>
@@ -8046,12 +8085,23 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
+        <v>89</v>
+      </c>
+      <c r="B87">
+        <v>7</v>
+      </c>
+      <c r="C87" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>90</v>
       </c>
-      <c r="B87">
+      <c r="B88">
         <v>3</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>4</v>
       </c>
     </row>
@@ -8062,31 +8112,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C678EEF9-365E-4FC0-9186-F5FC495503CF}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:XFD63"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>93</v>
@@ -8094,10 +8144,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>93</v>
@@ -8105,10 +8155,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>93</v>
@@ -8116,10 +8166,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>93</v>
@@ -8127,7 +8177,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -8138,10 +8188,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>93</v>
@@ -8149,7 +8199,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="B8">
         <v>9</v>
@@ -8160,10 +8210,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
         <v>93</v>
@@ -8171,7 +8221,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -8182,10 +8232,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>93</v>
@@ -8193,7 +8243,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -8204,10 +8254,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
         <v>93</v>
@@ -8215,10 +8265,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
         <v>93</v>
@@ -8226,7 +8276,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -8237,7 +8287,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -8248,7 +8298,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -8259,7 +8309,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -8270,10 +8320,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
         <v>93</v>
@@ -8281,7 +8331,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -8292,7 +8342,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -8303,7 +8353,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -8314,7 +8364,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -8325,7 +8375,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -8336,7 +8386,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -8347,7 +8397,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -8358,7 +8408,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -8369,10 +8419,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
         <v>93</v>
@@ -8380,7 +8430,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -8391,7 +8441,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -8402,7 +8452,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -8413,7 +8463,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -8424,7 +8474,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -8435,7 +8485,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -8446,7 +8496,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -8457,7 +8507,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -8468,7 +8518,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -8479,7 +8529,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -8490,7 +8540,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -8501,7 +8551,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -8512,7 +8562,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -8523,7 +8573,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -8534,7 +8584,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -8545,7 +8595,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -8556,7 +8606,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -8567,7 +8617,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -8578,7 +8628,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -8589,7 +8639,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -8600,7 +8650,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -8611,10 +8661,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50" t="s">
         <v>93</v>
@@ -8622,7 +8672,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -8633,7 +8683,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>11</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -8644,7 +8694,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -8655,7 +8705,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -8666,7 +8716,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -8677,7 +8727,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -8688,7 +8738,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -8699,7 +8749,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -8710,7 +8760,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -8721,7 +8771,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -8732,7 +8782,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -8743,12 +8793,23 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="C62" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>48</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>